<commit_message>
finish email sending auto
</commit_message>
<xml_diff>
--- a/Example/Example.xlsx
+++ b/Example/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangeethmenachery/Documents/Coding/pdf-generator/Example/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487E2162-065F-F148-8AD7-1EB393D01535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38B6314C-F782-3D42-8E7C-47AF8D7CD02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17160" xr2:uid="{05ECEB4F-11CE-B74F-940F-C3FEE0008888}"/>
   </bookViews>
@@ -110,7 +110,7 @@
     <t>Parent Email</t>
   </si>
   <si>
-    <t>sangeethmenachery@gmail.com, shijo_menachery@hotmail.com</t>
+    <t>sangeethmenachery@gmail.com, s@sangeethmenachery@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -981,7 +981,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>